<commit_message>
(feature/sdbDetails): join two tables in getbyid methods
</commit_message>
<xml_diff>
--- a/server/Uploads/BiaSODauBai.xlsx
+++ b/server/Uploads/BiaSODauBai.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenhu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenhu\OneDrive\Máy tính\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33180A5-150F-416F-9084-9CD2DA3D06BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C8976F-D945-4CE3-BC12-B66786EF6ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="2850" windowWidth="15615" windowHeight="11235" xr2:uid="{1B0A2674-79E5-4DCE-BF36-CBCFE2898E64}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{1B0A2674-79E5-4DCE-BF36-CBCFE2898E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,13 +428,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2D24B8-0224-4C66-830C-06867AC5AAEF}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -464,19 +473,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -484,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -492,31 +495,19 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -524,19 +515,13 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,19 +529,13 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -564,19 +543,13 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -584,19 +557,13 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -604,19 +571,13 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -624,19 +585,13 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -644,19 +599,265 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>